<commit_message>
Fix date import timezone conversion
</commit_message>
<xml_diff>
--- a/JosephM.Deployment.Test/Files/TestExcelImportAccountAndContact.xlsx
+++ b/JosephM.Deployment.Test/Files/TestExcelImportAccountAndContact.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>I Excel Account</t>
   </si>
@@ -46,13 +46,19 @@
   </si>
   <si>
     <t>Contact Company</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>lastonholdtime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +82,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -98,10 +110,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -383,19 +397,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -405,8 +422,14 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -415,6 +438,12 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" s="4">
+        <v>29540</v>
+      </c>
+      <c r="E2" s="4">
+        <v>29540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>